<commit_message>
Add name Komura Haruto
</commit_message>
<xml_diff>
--- a/Git_Challenge!!/NameList.xlsx
+++ b/Git_Challenge!!/NameList.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niwatakumi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doram\Documents\GitHub\NIT-Gifu_ComputerClub\Git_Challenge!!\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16584" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="NameList" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
     <phoneticPr fontId="2"/>
@@ -46,14 +46,22 @@
   </si>
   <si>
     <t>Welcome to ようこそ Github</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Komura Haruto</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>えいご wakarimasen</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,6 +119,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -379,19 +390,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.08984375" defaultRowHeight="19.8"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,17 +410,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>